<commit_message>
ng: add niger file
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_sites_june_06.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_sites_june_06.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E210DA1-4348-4009-963E-538FDE093DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF72A2F7-6B41-4149-BB4F-3E8ACF182B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B04231C6-1EC6-46D4-BFA8-7043CDC43D0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B04231C6-1EC6-46D4-BFA8-7043CDC43D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross River" sheetId="1" r:id="rId1"/>
     <sheet name="Bauchy" sheetId="2" r:id="rId2"/>
+    <sheet name="Niger" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="154">
   <si>
     <t>STATE</t>
   </si>
@@ -338,13 +339,172 @@
   </si>
   <si>
     <t>DISINA B</t>
+  </si>
+  <si>
+    <t>NIGER</t>
+  </si>
+  <si>
+    <t>AGAIE</t>
+  </si>
+  <si>
+    <t>AGWARA</t>
+  </si>
+  <si>
+    <t>BIDA</t>
+  </si>
+  <si>
+    <t>BORGU</t>
+  </si>
+  <si>
+    <t>GURARA</t>
+  </si>
+  <si>
+    <t>KATCHA</t>
+  </si>
+  <si>
+    <t>KONTAGORA</t>
+  </si>
+  <si>
+    <t>LAPAI</t>
+  </si>
+  <si>
+    <t>LAYUN</t>
+  </si>
+  <si>
+    <t>MAGAMA</t>
+  </si>
+  <si>
+    <t>MARIGA</t>
+  </si>
+  <si>
+    <t>MASHEGU</t>
+  </si>
+  <si>
+    <t>MUYA</t>
+  </si>
+  <si>
+    <t>RAFI</t>
+  </si>
+  <si>
+    <t>RIJUA</t>
+  </si>
+  <si>
+    <t>SHIRORO</t>
+  </si>
+  <si>
+    <t>WUSHISHI</t>
+  </si>
+  <si>
+    <t>MOKWA</t>
+  </si>
+  <si>
+    <t>BOSSO</t>
+  </si>
+  <si>
+    <t>EDATI</t>
+  </si>
+  <si>
+    <t>SONGUBI</t>
+  </si>
+  <si>
+    <t>BINUA</t>
+  </si>
+  <si>
+    <t>SCH. OF NURSING (BIDA)</t>
+  </si>
+  <si>
+    <t>BASE CAMP</t>
+  </si>
+  <si>
+    <t>DEKOLA</t>
+  </si>
+  <si>
+    <t>KANU</t>
+  </si>
+  <si>
+    <t>SHAFASHI</t>
+  </si>
+  <si>
+    <t>KWAKA</t>
+  </si>
+  <si>
+    <t>SHIRI</t>
+  </si>
+  <si>
+    <t>IBOLI</t>
+  </si>
+  <si>
+    <t>EBBO</t>
+  </si>
+  <si>
+    <t>KPOTGI</t>
+  </si>
+  <si>
+    <t>KUDUGI</t>
+  </si>
+  <si>
+    <t>ANABA</t>
+  </si>
+  <si>
+    <t>MORAIN KOTONKORO</t>
+  </si>
+  <si>
+    <t>CHEGU/LEABA</t>
+  </si>
+  <si>
+    <t>RIJIYAGI</t>
+  </si>
+  <si>
+    <t>ZUGUMA</t>
+  </si>
+  <si>
+    <t>WUCHI</t>
+  </si>
+  <si>
+    <t>KACHUWI</t>
+  </si>
+  <si>
+    <t>D'LADIMA</t>
+  </si>
+  <si>
+    <t>KWANGE</t>
+  </si>
+  <si>
+    <t>DUKU</t>
+  </si>
+  <si>
+    <t>WARARI</t>
+  </si>
+  <si>
+    <t>MADAKI</t>
+  </si>
+  <si>
+    <t>NDASSA</t>
+  </si>
+  <si>
+    <t>CHOGI</t>
+  </si>
+  <si>
+    <t>KASHUAN DAJI</t>
+  </si>
+  <si>
+    <t>KARENGI</t>
+  </si>
+  <si>
+    <t>HOUSES</t>
+  </si>
+  <si>
+    <t>KANGI TSUANPA</t>
+  </si>
+  <si>
+    <t>Site ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +535,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -390,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -413,21 +580,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1562,13 +1760,13 @@
     <sortCondition ref="L2:L33"/>
   </sortState>
   <conditionalFormatting sqref="C26:C1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:L33">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1579,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90B0466-1456-4310-B9D8-93C2D486B842}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C37"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,12 +2642,893 @@
     <sortCondition ref="L2:L38"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D980B132-FC94-4CEB-BFF9-C59D6EF6DD90}">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2">
+        <v>301</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3">
+        <v>302</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4">
+        <v>303</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5">
+        <v>304</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6">
+        <v>305</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7">
+        <v>306</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <v>307</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9">
+        <v>308</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10">
+        <v>309</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11">
+        <v>310</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12">
+        <v>311</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13">
+        <v>312</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14">
+        <v>313</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15">
+        <v>314</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16">
+        <v>315</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17">
+        <v>316</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18">
+        <v>317</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19">
+        <v>318</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20">
+        <v>319</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21">
+        <v>320</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22">
+        <v>321</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23">
+        <v>322</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24">
+        <v>323</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25">
+        <v>324</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26">
+        <v>325</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27">
+        <v>326</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28">
+        <v>327</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29">
+        <v>328</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30">
+        <v>329</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31">
+        <v>330</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32">
+        <v>331</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33">
+        <v>332</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34">
+        <v>333</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D35">
+        <v>334</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36">
+        <v>335</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K2:L40">
+    <sortCondition ref="K2:K40"/>
+    <sortCondition ref="L2:L40"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>